<commit_message>
update example output files
</commit_message>
<xml_diff>
--- a/EX3_ECG_samples/blink_record_align.xlsx
+++ b/EX3_ECG_samples/blink_record_align.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioxfordnexus.sharepoint.com/sites/ExperimentalPsychology-Leverhulme2022/Shared Documents/General/3_Data_Processing/Data_extraction/ECG_samples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexfraser/Development/example_code/EX3_ECG_samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{0C7BF57A-373A-4867-9E6A-47EE7C2882FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74C67CBE-A1DD-A540-9A48-0A2383F6CA37}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93FC87B2-1A76-AE49-8ED7-7203CBAF369E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="12220" xr2:uid="{5411588C-12F4-436F-BE8E-27D97ED59332}"/>
   </bookViews>
@@ -688,10 +688,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -994,7 +990,7 @@
   <dimension ref="A1:F173"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="C2" sqref="C2:C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1029,9 +1025,6 @@
       <c r="B2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="12">
-        <v>111</v>
-      </c>
       <c r="D2" s="19" t="s">
         <v>6</v>
       </c>
@@ -1046,9 +1039,7 @@
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="11">
-        <v>112</v>
-      </c>
+      <c r="C3" s="11"/>
       <c r="D3" s="8" t="s">
         <v>6</v>
       </c>
@@ -1066,9 +1057,7 @@
       <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="10">
-        <v>113</v>
-      </c>
+      <c r="C4" s="10"/>
       <c r="D4" s="8" t="s">
         <v>6</v>
       </c>
@@ -1083,9 +1072,7 @@
       <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="10">
-        <v>114</v>
-      </c>
+      <c r="C5" s="10"/>
       <c r="D5" s="8" t="s">
         <v>6</v>
       </c>
@@ -1100,9 +1087,7 @@
       <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="11">
-        <v>115</v>
-      </c>
+      <c r="C6" s="11"/>
       <c r="D6" s="20" t="s">
         <v>8</v>
       </c>
@@ -1117,9 +1102,7 @@
       <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="11">
-        <v>116</v>
-      </c>
+      <c r="C7" s="11"/>
       <c r="D7" s="8" t="s">
         <v>8</v>
       </c>
@@ -1134,9 +1117,7 @@
       <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="15">
-        <v>117</v>
-      </c>
+      <c r="C8" s="15"/>
       <c r="D8" s="21" t="s">
         <v>6</v>
       </c>
@@ -1151,9 +1132,7 @@
       <c r="B9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="16">
-        <v>118</v>
-      </c>
+      <c r="C9" s="16"/>
       <c r="D9" s="20" t="s">
         <v>8</v>
       </c>
@@ -1168,9 +1147,7 @@
       <c r="B10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="4">
-        <v>119</v>
-      </c>
+      <c r="C10" s="4"/>
       <c r="D10" s="22" t="s">
         <v>8</v>
       </c>
@@ -1185,9 +1162,7 @@
       <c r="B11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="4">
-        <v>120</v>
-      </c>
+      <c r="C11" s="4"/>
       <c r="D11" s="22" t="s">
         <v>8</v>
       </c>
@@ -1202,9 +1177,7 @@
       <c r="B12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="6">
-        <v>121</v>
-      </c>
+      <c r="C12" s="6"/>
       <c r="D12" s="6" t="s">
         <v>8</v>
       </c>
@@ -1219,9 +1192,7 @@
       <c r="B13" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="7">
-        <v>122</v>
-      </c>
+      <c r="C13" s="7"/>
       <c r="D13" s="17" t="s">
         <v>8</v>
       </c>
@@ -1236,9 +1207,7 @@
       <c r="B14" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="13">
-        <v>123</v>
-      </c>
+      <c r="C14" s="13"/>
       <c r="D14" s="23" t="s">
         <v>8</v>
       </c>
@@ -1253,9 +1222,7 @@
       <c r="B15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="4">
-        <v>124</v>
-      </c>
+      <c r="C15" s="4"/>
       <c r="D15" s="22" t="s">
         <v>6</v>
       </c>
@@ -1270,9 +1237,7 @@
       <c r="B16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="4">
-        <v>125</v>
-      </c>
+      <c r="C16" s="4"/>
       <c r="D16" s="22" t="s">
         <v>8</v>
       </c>
@@ -1287,9 +1252,7 @@
       <c r="B17" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="4">
-        <v>126</v>
-      </c>
+      <c r="C17" s="4"/>
       <c r="D17" s="22" t="s">
         <v>8</v>
       </c>
@@ -1304,9 +1267,7 @@
       <c r="B18" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="4">
-        <v>127</v>
-      </c>
+      <c r="C18" s="4"/>
       <c r="D18" s="22" t="s">
         <v>8</v>
       </c>
@@ -1321,9 +1282,7 @@
       <c r="B19" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="4">
-        <v>128</v>
-      </c>
+      <c r="C19" s="4"/>
       <c r="D19" s="22" t="s">
         <v>6</v>
       </c>
@@ -1338,9 +1297,7 @@
       <c r="B20" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="4">
-        <v>129</v>
-      </c>
+      <c r="C20" s="4"/>
       <c r="D20" s="22" t="s">
         <v>6</v>
       </c>
@@ -1355,9 +1312,7 @@
       <c r="B21" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="5">
-        <v>130</v>
-      </c>
+      <c r="C21" s="5"/>
       <c r="D21" s="6" t="s">
         <v>8</v>
       </c>
@@ -1372,9 +1327,7 @@
       <c r="B22" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="3">
-        <v>131</v>
-      </c>
+      <c r="C22" s="3"/>
       <c r="D22" s="20" t="s">
         <v>6</v>
       </c>
@@ -1389,9 +1342,7 @@
       <c r="B23" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="3">
-        <v>132</v>
-      </c>
+      <c r="C23" s="3"/>
       <c r="D23" s="20" t="s">
         <v>8</v>
       </c>
@@ -1406,9 +1357,7 @@
       <c r="B24" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="3">
-        <v>133</v>
-      </c>
+      <c r="C24" s="3"/>
       <c r="D24" s="3" t="s">
         <v>8</v>
       </c>
@@ -1423,9 +1372,7 @@
       <c r="B25" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="2">
-        <v>134</v>
-      </c>
+      <c r="C25" s="2"/>
       <c r="D25" s="20" t="s">
         <v>6</v>
       </c>
@@ -1440,9 +1387,7 @@
       <c r="B26" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="3">
-        <v>135</v>
-      </c>
+      <c r="C26" s="3"/>
       <c r="D26" s="20" t="s">
         <v>8</v>
       </c>
@@ -1457,9 +1402,7 @@
       <c r="B27" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="2">
-        <v>136</v>
-      </c>
+      <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
         <v>8</v>
       </c>
@@ -1474,9 +1417,7 @@
       <c r="B28" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="8">
-        <v>137</v>
-      </c>
+      <c r="C28" s="8"/>
       <c r="D28" s="8" t="s">
         <v>8</v>
       </c>
@@ -1491,9 +1432,7 @@
       <c r="B29" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="2">
-        <v>138</v>
-      </c>
+      <c r="C29" s="2"/>
       <c r="D29" s="8" t="s">
         <v>8</v>
       </c>
@@ -1508,9 +1447,7 @@
       <c r="B30" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="2">
-        <v>139</v>
-      </c>
+      <c r="C30" s="2"/>
       <c r="D30" s="8" t="s">
         <v>8</v>
       </c>
@@ -1525,9 +1462,7 @@
       <c r="B31" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="2">
-        <v>140</v>
-      </c>
+      <c r="C31" s="2"/>
       <c r="D31" s="8" t="s">
         <v>8</v>
       </c>
@@ -1542,9 +1477,7 @@
       <c r="B32" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="2">
-        <v>141</v>
-      </c>
+      <c r="C32" s="2"/>
       <c r="D32" s="8" t="s">
         <v>6</v>
       </c>
@@ -1559,9 +1492,7 @@
       <c r="B33" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="2">
-        <v>142</v>
-      </c>
+      <c r="C33" s="2"/>
       <c r="D33" s="8" t="s">
         <v>8</v>
       </c>
@@ -1576,9 +1507,7 @@
       <c r="B34" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="3">
-        <v>143</v>
-      </c>
+      <c r="C34" s="3"/>
       <c r="D34" s="20" t="s">
         <v>6</v>
       </c>
@@ -1593,9 +1522,7 @@
       <c r="B35" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="17">
-        <v>144</v>
-      </c>
+      <c r="C35" s="17"/>
       <c r="D35" s="8" t="s">
         <v>8</v>
       </c>
@@ -1610,9 +1537,7 @@
       <c r="B36" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C36" s="2">
-        <v>145</v>
-      </c>
+      <c r="C36" s="2"/>
       <c r="D36" s="8" t="s">
         <v>8</v>
       </c>
@@ -1627,9 +1552,7 @@
       <c r="B37" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C37" s="2">
-        <v>146</v>
-      </c>
+      <c r="C37" s="2"/>
       <c r="D37" s="8" t="s">
         <v>6</v>
       </c>
@@ -1644,9 +1567,7 @@
       <c r="B38" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="2">
-        <v>147</v>
-      </c>
+      <c r="C38" s="2"/>
       <c r="D38" s="8" t="s">
         <v>8</v>
       </c>
@@ -1661,9 +1582,7 @@
       <c r="B39" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C39" s="2">
-        <v>148</v>
-      </c>
+      <c r="C39" s="2"/>
       <c r="D39" s="8" t="s">
         <v>49</v>
       </c>
@@ -1678,9 +1597,7 @@
       <c r="B40" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C40" s="2">
-        <v>149</v>
-      </c>
+      <c r="C40" s="2"/>
       <c r="D40" s="8" t="s">
         <v>8</v>
       </c>
@@ -1695,9 +1612,7 @@
       <c r="B41" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C41" s="2">
-        <v>150</v>
-      </c>
+      <c r="C41" s="2"/>
       <c r="D41" s="8" t="s">
         <v>8</v>
       </c>
@@ -1712,9 +1627,7 @@
       <c r="B42" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C42" s="2">
-        <v>151</v>
-      </c>
+      <c r="C42" s="2"/>
       <c r="D42" s="8" t="s">
         <v>8</v>
       </c>
@@ -1729,9 +1642,7 @@
       <c r="B43" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C43" s="2">
-        <v>152</v>
-      </c>
+      <c r="C43" s="2"/>
       <c r="D43" s="8" t="s">
         <v>8</v>
       </c>
@@ -1746,9 +1657,7 @@
       <c r="B44" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C44" s="2">
-        <v>153</v>
-      </c>
+      <c r="C44" s="2"/>
       <c r="D44" s="8" t="s">
         <v>8</v>
       </c>
@@ -1763,9 +1672,7 @@
       <c r="B45" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C45" s="2">
-        <v>154</v>
-      </c>
+      <c r="C45" s="2"/>
       <c r="D45" s="8" t="s">
         <v>55</v>
       </c>
@@ -1780,9 +1687,7 @@
       <c r="B46" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C46" s="2">
-        <v>155</v>
-      </c>
+      <c r="C46" s="2"/>
       <c r="D46" s="8" t="s">
         <v>8</v>
       </c>
@@ -1797,9 +1702,7 @@
       <c r="B47" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C47" s="2">
-        <v>156</v>
-      </c>
+      <c r="C47" s="2"/>
       <c r="D47" s="8" t="s">
         <v>60</v>
       </c>
@@ -1812,9 +1715,7 @@
         <v>61</v>
       </c>
       <c r="B48" s="2"/>
-      <c r="C48" s="2">
-        <v>157</v>
-      </c>
+      <c r="C48" s="2"/>
       <c r="D48" s="8" t="s">
         <v>8</v>
       </c>
@@ -1829,9 +1730,7 @@
       <c r="B49" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C49" s="2">
-        <v>158</v>
-      </c>
+      <c r="C49" s="2"/>
       <c r="D49" s="8" t="s">
         <v>8</v>
       </c>
@@ -1846,9 +1745,7 @@
       <c r="B50" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C50" s="2">
-        <v>159</v>
-      </c>
+      <c r="C50" s="2"/>
       <c r="D50" s="2" t="s">
         <v>8</v>
       </c>
@@ -1863,9 +1760,7 @@
       <c r="B51" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C51" s="2">
-        <v>160</v>
-      </c>
+      <c r="C51" s="2"/>
       <c r="D51" s="8" t="s">
         <v>6</v>
       </c>
@@ -1880,9 +1775,7 @@
       <c r="B52" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="C52" s="2">
-        <v>161</v>
-      </c>
+      <c r="C52" s="2"/>
       <c r="D52" s="8" t="s">
         <v>60</v>
       </c>
@@ -1897,9 +1790,7 @@
       <c r="B53" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C53" s="2">
-        <v>162</v>
-      </c>
+      <c r="C53" s="2"/>
       <c r="D53" s="8" t="s">
         <v>60</v>
       </c>
@@ -1914,9 +1805,7 @@
       <c r="B54" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C54" s="2">
-        <v>163</v>
-      </c>
+      <c r="C54" s="2"/>
       <c r="D54" s="8" t="s">
         <v>60</v>
       </c>
@@ -1931,9 +1820,7 @@
       <c r="B55" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C55" s="2">
-        <v>164</v>
-      </c>
+      <c r="C55" s="2"/>
       <c r="D55" s="8" t="s">
         <v>60</v>
       </c>
@@ -1948,9 +1835,7 @@
       <c r="B56" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C56" s="2">
-        <v>165</v>
-      </c>
+      <c r="C56" s="2"/>
       <c r="D56" s="8" t="s">
         <v>8</v>
       </c>
@@ -1965,9 +1850,7 @@
       <c r="B57" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C57" s="2">
-        <v>166</v>
-      </c>
+      <c r="C57" s="2"/>
       <c r="D57" s="8" t="s">
         <v>8</v>
       </c>
@@ -1982,9 +1865,7 @@
       <c r="B58" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C58" s="2">
-        <v>167</v>
-      </c>
+      <c r="C58" s="2"/>
       <c r="D58" s="8" t="s">
         <v>8</v>
       </c>
@@ -1999,9 +1880,7 @@
       <c r="B59" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C59" s="2">
-        <v>168</v>
-      </c>
+      <c r="C59" s="2"/>
       <c r="D59" s="8" t="s">
         <v>8</v>
       </c>
@@ -2016,9 +1895,7 @@
       <c r="B60" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C60" s="2">
-        <v>169</v>
-      </c>
+      <c r="C60" s="2"/>
       <c r="D60" s="8" t="s">
         <v>8</v>
       </c>
@@ -2033,9 +1910,7 @@
       <c r="B61" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C61" s="2">
-        <v>170</v>
-      </c>
+      <c r="C61" s="2"/>
       <c r="D61" s="8" t="s">
         <v>8</v>
       </c>
@@ -2050,9 +1925,7 @@
       <c r="B62" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C62" s="2">
-        <v>171</v>
-      </c>
+      <c r="C62" s="2"/>
       <c r="D62" s="8" t="s">
         <v>6</v>
       </c>
@@ -2067,9 +1940,7 @@
       <c r="B63" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C63" s="2">
-        <v>172</v>
-      </c>
+      <c r="C63" s="2"/>
       <c r="D63" s="8" t="s">
         <v>8</v>
       </c>
@@ -2084,9 +1955,7 @@
       <c r="B64" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C64" s="2">
-        <v>173</v>
-      </c>
+      <c r="C64" s="2"/>
       <c r="D64" s="8" t="s">
         <v>8</v>
       </c>
@@ -2101,9 +1970,7 @@
       <c r="B65" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C65" s="2">
-        <v>174</v>
-      </c>
+      <c r="C65" s="2"/>
       <c r="D65" s="8" t="s">
         <v>80</v>
       </c>
@@ -2118,9 +1985,7 @@
       <c r="B66" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C66" s="2">
-        <v>175</v>
-      </c>
+      <c r="C66" s="2"/>
       <c r="D66" s="8" t="s">
         <v>8</v>
       </c>
@@ -2135,9 +2000,7 @@
       <c r="B67" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C67" s="2">
-        <v>176</v>
-      </c>
+      <c r="C67" s="2"/>
       <c r="D67" s="8" t="s">
         <v>6</v>
       </c>
@@ -2152,9 +2015,7 @@
       <c r="B68" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C68" s="2">
-        <v>177</v>
-      </c>
+      <c r="C68" s="2"/>
       <c r="D68" s="8" t="s">
         <v>8</v>
       </c>
@@ -2169,9 +2030,7 @@
       <c r="B69" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C69" s="2">
-        <v>178</v>
-      </c>
+      <c r="C69" s="2"/>
       <c r="D69" s="8" t="s">
         <v>8</v>
       </c>
@@ -2186,9 +2045,7 @@
       <c r="B70" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C70" s="2">
-        <v>179</v>
-      </c>
+      <c r="C70" s="2"/>
       <c r="D70" s="8"/>
       <c r="E70" s="8"/>
     </row>
@@ -2199,9 +2056,7 @@
       <c r="B71" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C71" s="2">
-        <v>179</v>
-      </c>
+      <c r="C71" s="2"/>
       <c r="D71" s="8" t="s">
         <v>8</v>
       </c>
@@ -2216,9 +2071,7 @@
       <c r="B72" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C72" s="2">
-        <v>180</v>
-      </c>
+      <c r="C72" s="2"/>
       <c r="D72" s="8"/>
       <c r="E72" s="8"/>
     </row>
@@ -2229,9 +2082,7 @@
       <c r="B73" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C73" s="2">
-        <v>180</v>
-      </c>
+      <c r="C73" s="2"/>
       <c r="D73" s="8" t="s">
         <v>8</v>
       </c>
@@ -2246,9 +2097,7 @@
       <c r="B74" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C74" s="2">
-        <v>181</v>
-      </c>
+      <c r="C74" s="2"/>
       <c r="D74" s="8" t="s">
         <v>8</v>
       </c>
@@ -2263,9 +2112,7 @@
       <c r="B75" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C75" s="2">
-        <v>182</v>
-      </c>
+      <c r="C75" s="2"/>
       <c r="D75" s="8" t="s">
         <v>8</v>
       </c>
@@ -2280,9 +2127,7 @@
       <c r="B76" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C76" s="2">
-        <v>183</v>
-      </c>
+      <c r="C76" s="2"/>
       <c r="D76" s="8" t="s">
         <v>60</v>
       </c>
@@ -2297,9 +2142,7 @@
       <c r="B77" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C77" s="2">
-        <v>184</v>
-      </c>
+      <c r="C77" s="2"/>
       <c r="D77" s="8" t="s">
         <v>8</v>
       </c>
@@ -2314,9 +2157,7 @@
       <c r="B78" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C78" s="2">
-        <v>185</v>
-      </c>
+      <c r="C78" s="2"/>
       <c r="D78" s="8" t="s">
         <v>8</v>
       </c>
@@ -2331,9 +2172,7 @@
       <c r="B79" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C79" s="2">
-        <v>186</v>
-      </c>
+      <c r="C79" s="2"/>
       <c r="D79" s="8" t="s">
         <v>8</v>
       </c>
@@ -2348,9 +2187,7 @@
       <c r="B80" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C80" s="2">
-        <v>187</v>
-      </c>
+      <c r="C80" s="2"/>
       <c r="D80" s="8" t="s">
         <v>6</v>
       </c>
@@ -2365,9 +2202,7 @@
       <c r="B81" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C81" s="2">
-        <v>188</v>
-      </c>
+      <c r="C81" s="2"/>
       <c r="D81" s="8" t="s">
         <v>6</v>
       </c>
@@ -2946,15 +2781,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="c7b00679-b217-4836-acbb-86e4d62c5d4d" xsi:nil="true"/>
@@ -2963,6 +2789,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3215,14 +3050,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDB0293C-8FFB-4049-BA92-14F917100DE8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22B0240E-E9C4-4BF0-B582-78F161DB93D3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -3235,6 +3062,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDB0293C-8FFB-4049-BA92-14F917100DE8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>